<commit_message>
REPORTGEN-1053: update chinese templates
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/zh-CN/Application/Compliance reports/ISO-5055 全部详细报告.xlsx
+++ b/CastReporting.Reporting.Core/Templates/zh-CN/Application/Compliance reports/ISO-5055 全部详细报告.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwang/Documents/Localization/RG-Templates/ISO-5055-TemplateToTranslate/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\zh-CN\Application\Compliance reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C58E2A-8018-904C-B571-9BFEDDC4B584}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BBF846-0E1D-4629-B2E1-445A0CA561CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="概述" sheetId="6" r:id="rId1"/>
@@ -59,9 +59,6 @@
     <t>RepGen:TEXT;LAST_SNAPSHOT_DATE</t>
   </si>
   <si>
-    <t>RepGen:TEXT;METRIC_TECHNICAL_DEBT</t>
-  </si>
-  <si>
     <t>RepGen:TABLE;TECHNO_LOC;HEADER=NO</t>
   </si>
   <si>
@@ -226,19 +223,22 @@
     </r>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
+  <si>
+    <t>RepGen:TEXT;OMG_TECHNICAL_DEBT</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="0&quot; LoC&quot;"/>
+    <numFmt numFmtId="164" formatCode="0&quot; LoC&quot;"/>
   </numFmts>
   <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -253,7 +253,7 @@
       <b/>
       <sz val="16"/>
       <color indexed="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -268,14 +268,14 @@
       <b/>
       <sz val="11"/>
       <color indexed="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -283,7 +283,7 @@
       <b/>
       <sz val="18"/>
       <color indexed="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -291,7 +291,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -311,7 +311,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -501,7 +501,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -534,22 +534,22 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Header 1" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -925,38 +925,38 @@
   <dimension ref="B1:O14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.5" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" customWidth="1"/>
     <col min="2" max="2" width="66" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" customWidth="1"/>
-    <col min="6" max="6" width="16.1640625" customWidth="1"/>
-    <col min="7" max="7" width="19.5" customWidth="1"/>
-    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" customWidth="1"/>
-    <col min="13" max="13" width="36.6640625" customWidth="1"/>
-    <col min="14" max="14" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1"/>
+    <col min="13" max="13" width="36.7109375" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15" thickBot="1">
+    <row r="1" spans="2:15" ht="15.75" thickBot="1">
       <c r="D1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-    </row>
-    <row r="2" spans="2:15" ht="24">
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+    </row>
+    <row r="2" spans="2:15" ht="23.25">
       <c r="B2" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="2"/>
@@ -966,7 +966,7 @@
     </row>
     <row r="3" spans="2:15" ht="15" customHeight="1">
       <c r="B3" s="21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>0</v>
@@ -974,7 +974,7 @@
       <c r="D3" s="11"/>
       <c r="E3" s="12"/>
       <c r="F3" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G3" s="15" t="s">
         <v>1</v>
@@ -982,7 +982,7 @@
     </row>
     <row r="4" spans="2:15" ht="15" customHeight="1" thickBot="1">
       <c r="B4" s="22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>3</v>
@@ -990,10 +990,10 @@
       <c r="D4" s="4"/>
       <c r="E4" s="13"/>
       <c r="F4" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="2:15" ht="14.25" customHeight="1">
@@ -1001,32 +1001,32 @@
     </row>
     <row r="6" spans="2:15">
       <c r="B6" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="D6" s="18" t="s">
         <v>23</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="7" spans="2:15">
       <c r="C7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7" s="23"/>
     </row>
     <row r="8" spans="2:15">
       <c r="C8" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="18" t="s">
         <v>25</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="9" spans="2:15">
       <c r="C9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D9" s="23"/>
       <c r="N9" s="17"/>
@@ -1034,26 +1034,26 @@
     </row>
     <row r="12" spans="2:15">
       <c r="B12" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="2:15">
       <c r="B13" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="D13" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="E13" s="27" t="s">
         <v>30</v>
-      </c>
-      <c r="E13" s="28" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="14" spans="2:15">
       <c r="B14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14" s="23"/>
       <c r="D14" s="23"/>
@@ -1078,43 +1078,43 @@
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="88.33203125" customWidth="1"/>
-    <col min="2" max="2" width="24.5" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.83203125" customWidth="1"/>
-    <col min="6" max="6" width="42.33203125" customWidth="1"/>
-    <col min="7" max="7" width="44.6640625" customWidth="1"/>
+    <col min="1" max="1" width="88.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.85546875" customWidth="1"/>
+    <col min="6" max="6" width="42.28515625" customWidth="1"/>
+    <col min="7" max="7" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="20" t="s">
+      <c r="F1" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="G1" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="30" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15">
+    </row>
+    <row r="2" spans="1:7" ht="30">
       <c r="A2" s="25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
@@ -1138,47 +1138,47 @@
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="94" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="58.83203125" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="H1" s="20" t="s">
         <v>33</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1196,43 +1196,43 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="89.33203125" customWidth="1"/>
-    <col min="2" max="2" width="24.5" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.83203125" customWidth="1"/>
-    <col min="6" max="6" width="42.33203125" customWidth="1"/>
-    <col min="7" max="7" width="44.6640625" customWidth="1"/>
+    <col min="1" max="1" width="89.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.85546875" customWidth="1"/>
+    <col min="6" max="6" width="42.28515625" customWidth="1"/>
+    <col min="7" max="7" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="20" t="s">
+      <c r="F1" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="G1" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="30" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15">
+    </row>
+    <row r="2" spans="1:7" ht="30">
       <c r="A2" s="25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
@@ -1256,47 +1256,47 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="94" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="58.83203125" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="H1" s="20" t="s">
         <v>33</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1314,43 +1314,43 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="101" customWidth="1"/>
-    <col min="2" max="2" width="24.5" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.83203125" customWidth="1"/>
-    <col min="6" max="6" width="42.33203125" customWidth="1"/>
-    <col min="7" max="7" width="44.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.85546875" customWidth="1"/>
+    <col min="6" max="6" width="42.28515625" customWidth="1"/>
+    <col min="7" max="7" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="20" t="s">
+      <c r="F1" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="G1" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="30" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15">
+    </row>
+    <row r="2" spans="1:7" ht="30">
       <c r="A2" s="25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
@@ -1374,47 +1374,47 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="94" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="58.83203125" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="H1" s="20" t="s">
         <v>33</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1432,43 +1432,43 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="93.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.83203125" customWidth="1"/>
-    <col min="6" max="6" width="42.33203125" customWidth="1"/>
-    <col min="7" max="7" width="44.6640625" customWidth="1"/>
+    <col min="1" max="1" width="93.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.85546875" customWidth="1"/>
+    <col min="6" max="6" width="42.28515625" customWidth="1"/>
+    <col min="7" max="7" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="20" t="s">
+      <c r="F1" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="G1" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="30" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15">
+    </row>
+    <row r="2" spans="1:7" ht="30">
       <c r="A2" s="25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
@@ -1492,47 +1492,47 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="94" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="58.83203125" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="H1" s="20" t="s">
         <v>33</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>